<commit_message>
fix label to Netherlands
</commit_message>
<xml_diff>
--- a/data-raw/days_365/days_365.xlsx
+++ b/data-raw/days_365/days_365.xlsx
@@ -419,7 +419,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -448,7 +448,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -622,7 +622,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -680,7 +680,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -709,7 +709,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -738,7 +738,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -767,7 +767,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -796,7 +796,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -883,7 +883,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -970,7 +970,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -999,7 +999,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1202,7 +1202,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1724,7 +1724,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1840,7 +1840,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1898,7 +1898,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2072,7 +2072,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2130,7 +2130,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2188,7 +2188,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2420,7 +2420,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2507,7 +2507,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2594,7 +2594,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2623,7 +2623,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2855,7 +2855,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2884,7 +2884,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2942,7 +2942,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -3029,7 +3029,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>

</xml_diff>